<commit_message>
* conver to json
</commit_message>
<xml_diff>
--- a/Assets/Test/Test4.xlsx
+++ b/Assets/Test/Test4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="25605" windowHeight="15165"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="25605" windowHeight="15165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -47,6 +47,38 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Name1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name6</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name7</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name8</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -445,7 +477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -819,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,28 +868,28 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="K1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>